<commit_message>
make script read google spreadsheet & update finish conditions
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B2E4C5-2C81-4237-805D-9665D43C337E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF42317-06E7-445B-A4B7-07FA0D95C945}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ui" sheetId="10" r:id="rId1"/>
@@ -15,7 +15,8 @@
     <sheet name="event_cards" sheetId="7" r:id="rId5"/>
     <sheet name="player_cards" sheetId="8" r:id="rId6"/>
     <sheet name="tile_info" sheetId="11" r:id="rId7"/>
-    <sheet name="s_scavenge_vs_gather" sheetId="9" r:id="rId8"/>
+    <sheet name="players" sheetId="12" r:id="rId8"/>
+    <sheet name="s_scavenge_vs_gather" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="buildable" localSheetId="4">#REF!</definedName>
@@ -844,6 +845,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -853,8 +856,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3756,7 +3757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A9D0752-48DF-4D45-B912-C3CDBBD6BD64}">
   <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
@@ -4273,15 +4274,15 @@
       <c r="O11" s="11"/>
       <c r="P11" s="42">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q11" s="43">
         <f t="shared" ref="Q11:Q12" ca="1" si="0">RANDBETWEEN(1,6)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="R11" s="44">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="V11" s="12"/>
     </row>
@@ -4331,11 +4332,11 @@
       <c r="O12" s="11"/>
       <c r="P12" s="42">
         <f t="shared" ref="P12:P14" ca="1" si="1">RANDBETWEEN(1,6)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q12" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R12" s="45"/>
       <c r="V12" s="12"/>
@@ -4386,7 +4387,7 @@
       <c r="O13" s="11"/>
       <c r="P13" s="42">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="Q13" s="46"/>
       <c r="R13" s="45"/>
@@ -4438,7 +4439,7 @@
       <c r="O14" s="11"/>
       <c r="P14" s="47">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q14" s="18"/>
       <c r="R14" s="48"/>
@@ -4722,7 +4723,7 @@
   <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:Q10"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5527,25 +5528,25 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
       <c r="J1" s="12"/>
-      <c r="K1" s="55" t="s">
+      <c r="K1" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
     </row>
     <row r="2" spans="1:21" s="8" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
@@ -6719,7 +6720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAFA5479-08DC-4BDE-863C-D0D511EB4A48}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -6732,10 +6733,10 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="56" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="56" t="s">
         <v>142</v>
       </c>
     </row>
@@ -6746,10 +6747,10 @@
       <c r="B2" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="55" t="s">
         <v>58</v>
       </c>
     </row>
@@ -6760,10 +6761,10 @@
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="55" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="55" t="s">
         <v>59</v>
       </c>
     </row>
@@ -6774,10 +6775,10 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="55" t="s">
         <v>60</v>
       </c>
     </row>
@@ -6788,10 +6789,10 @@
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="58" t="s">
+      <c r="D5" s="55" t="s">
         <v>61</v>
       </c>
     </row>
@@ -6802,10 +6803,10 @@
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="58" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" s="58" t="s">
+      <c r="C6" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="55" t="s">
         <v>62</v>
       </c>
     </row>
@@ -6816,10 +6817,10 @@
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="D7" s="58" t="s">
+      <c r="D7" s="55" t="s">
         <v>140</v>
       </c>
     </row>
@@ -6830,10 +6831,10 @@
       <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="58" t="s">
+      <c r="C8" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="58" t="s">
+      <c r="D8" s="55" t="s">
         <v>141</v>
       </c>
     </row>
@@ -6844,10 +6845,10 @@
       <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="C9" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="58" t="s">
+      <c r="D9" s="55" t="s">
         <v>63</v>
       </c>
     </row>
@@ -6857,10 +6858,1359 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F9689DF-8423-4ED6-A8C3-450F68754E16}">
+  <dimension ref="A1:N23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" t="str">
+        <f>IF(ISBLANK(ui!A15),"",ui!A15)</f>
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <f>IF(ISBLANK(ui!B15),"",ui!B15)</f>
+        <v>name</v>
+      </c>
+      <c r="C1" t="str">
+        <f>IF(ISBLANK(ui!C15),"",ui!C15)</f>
+        <v>survivors</v>
+      </c>
+      <c r="D1" t="str">
+        <f>IF(ISBLANK(ui!D15),"",ui!D15)</f>
+        <v>water</v>
+      </c>
+      <c r="E1" t="str">
+        <f>IF(ISBLANK(ui!E15),"",ui!E15)</f>
+        <v>food</v>
+      </c>
+      <c r="F1" t="str">
+        <f>IF(ISBLANK(ui!F15),"",ui!F15)</f>
+        <v>medicines</v>
+      </c>
+      <c r="G1" t="str">
+        <f>IF(ISBLANK(ui!G15),"",ui!G15)</f>
+        <v>rock</v>
+      </c>
+      <c r="H1" t="str">
+        <f>IF(ISBLANK(ui!H15),"",ui!H15)</f>
+        <v>wood</v>
+      </c>
+      <c r="I1" t="str">
+        <f>IF(ISBLANK(ui!I15),"",ui!I15)</f>
+        <v>tools</v>
+      </c>
+      <c r="J1" t="str">
+        <f>IF(ISBLANK(ui!J15),"",ui!J15)</f>
+        <v>weapons</v>
+      </c>
+      <c r="K1" t="str">
+        <f>IF(ISBLANK(ui!K15),"",ui!K15)</f>
+        <v>information</v>
+      </c>
+      <c r="L1" t="str">
+        <f>IF(ISBLANK(ui!L15),"",ui!L15)</f>
+        <v>wounded</v>
+      </c>
+      <c r="M1" t="str">
+        <f>IF(ISBLANK(ui!M15),"",ui!M15)</f>
+        <v>idlers</v>
+      </c>
+      <c r="N1" t="str">
+        <f>IF(ISBLANK(ui!N15),"",ui!N15)</f>
+        <v>points</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <f>IF(ISBLANK(ui!A16),"",ui!A16)</f>
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <f>IF(ISBLANK(ui!B16),"",ui!B16)</f>
+        <v>Imanol</v>
+      </c>
+      <c r="C2">
+        <f>IF(ISBLANK(ui!C16),"",ui!C16)</f>
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <f>IF(ISBLANK(ui!D16),"",ui!D16)</f>
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <f>IF(ISBLANK(ui!E16),"",ui!E16)</f>
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <f>IF(ISBLANK(ui!F16),"",ui!F16)</f>
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <f>IF(ISBLANK(ui!G16),"",ui!G16)</f>
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <f>IF(ISBLANK(ui!H16),"",ui!H16)</f>
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <f>IF(ISBLANK(ui!I16),"",ui!I16)</f>
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <f>IF(ISBLANK(ui!J16),"",ui!J16)</f>
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <f>IF(ISBLANK(ui!K16),"",ui!K16)</f>
+        <v>5</v>
+      </c>
+      <c r="L2">
+        <f>IF(ISBLANK(ui!L16),"",ui!L16)</f>
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <f>IF(ISBLANK(ui!M16),"",ui!M16)</f>
+        <v>3</v>
+      </c>
+      <c r="N2">
+        <f>IF(ISBLANK(ui!N16),"",ui!N16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>IF(ISBLANK(ui!A17),"",ui!A17)</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <f>IF(ISBLANK(ui!B17),"",ui!B17)</f>
+        <v>Anna</v>
+      </c>
+      <c r="C3">
+        <f>IF(ISBLANK(ui!C17),"",ui!C17)</f>
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <f>IF(ISBLANK(ui!D17),"",ui!D17)</f>
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <f>IF(ISBLANK(ui!E17),"",ui!E17)</f>
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <f>IF(ISBLANK(ui!F17),"",ui!F17)</f>
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <f>IF(ISBLANK(ui!G17),"",ui!G17)</f>
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <f>IF(ISBLANK(ui!H17),"",ui!H17)</f>
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <f>IF(ISBLANK(ui!I17),"",ui!I17)</f>
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <f>IF(ISBLANK(ui!J17),"",ui!J17)</f>
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f>IF(ISBLANK(ui!K17),"",ui!K17)</f>
+        <v>5</v>
+      </c>
+      <c r="L3">
+        <f>IF(ISBLANK(ui!L17),"",ui!L17)</f>
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <f>IF(ISBLANK(ui!M17),"",ui!M17)</f>
+        <v>3</v>
+      </c>
+      <c r="N3">
+        <f>IF(ISBLANK(ui!N17),"",ui!N17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f>IF(ISBLANK(ui!A18),"",ui!A18)</f>
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f>IF(ISBLANK(ui!B18),"",ui!B18)</f>
+        <v>Kaija</v>
+      </c>
+      <c r="C4">
+        <f>IF(ISBLANK(ui!C18),"",ui!C18)</f>
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <f>IF(ISBLANK(ui!D18),"",ui!D18)</f>
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <f>IF(ISBLANK(ui!E18),"",ui!E18)</f>
+        <v>9</v>
+      </c>
+      <c r="F4">
+        <f>IF(ISBLANK(ui!F18),"",ui!F18)</f>
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <f>IF(ISBLANK(ui!G18),"",ui!G18)</f>
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <f>IF(ISBLANK(ui!H18),"",ui!H18)</f>
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <f>IF(ISBLANK(ui!I18),"",ui!I18)</f>
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <f>IF(ISBLANK(ui!J18),"",ui!J18)</f>
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f>IF(ISBLANK(ui!K18),"",ui!K18)</f>
+        <v>5</v>
+      </c>
+      <c r="L4">
+        <f>IF(ISBLANK(ui!L18),"",ui!L18)</f>
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f>IF(ISBLANK(ui!M18),"",ui!M18)</f>
+        <v>3</v>
+      </c>
+      <c r="N4">
+        <f>IF(ISBLANK(ui!N18),"",ui!N18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f>IF(ISBLANK(ui!A19),"",ui!A19)</f>
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <f>IF(ISBLANK(ui!B19),"",ui!B19)</f>
+        <v>Igor</v>
+      </c>
+      <c r="C5">
+        <f>IF(ISBLANK(ui!C19),"",ui!C19)</f>
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <f>IF(ISBLANK(ui!D19),"",ui!D19)</f>
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <f>IF(ISBLANK(ui!E19),"",ui!E19)</f>
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <f>IF(ISBLANK(ui!F19),"",ui!F19)</f>
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <f>IF(ISBLANK(ui!G19),"",ui!G19)</f>
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <f>IF(ISBLANK(ui!H19),"",ui!H19)</f>
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <f>IF(ISBLANK(ui!I19),"",ui!I19)</f>
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <f>IF(ISBLANK(ui!J19),"",ui!J19)</f>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f>IF(ISBLANK(ui!K19),"",ui!K19)</f>
+        <v>5</v>
+      </c>
+      <c r="L5">
+        <f>IF(ISBLANK(ui!L19),"",ui!L19)</f>
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <f>IF(ISBLANK(ui!M19),"",ui!M19)</f>
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <f>IF(ISBLANK(ui!N19),"",ui!N19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f>IF(ISBLANK(ui!A20),"",ui!A20)</f>
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <f>IF(ISBLANK(ui!B20),"",ui!B20)</f>
+        <v>Caroline</v>
+      </c>
+      <c r="C6">
+        <f>IF(ISBLANK(ui!C20),"",ui!C20)</f>
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <f>IF(ISBLANK(ui!D20),"",ui!D20)</f>
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <f>IF(ISBLANK(ui!E20),"",ui!E20)</f>
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <f>IF(ISBLANK(ui!F20),"",ui!F20)</f>
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <f>IF(ISBLANK(ui!G20),"",ui!G20)</f>
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <f>IF(ISBLANK(ui!H20),"",ui!H20)</f>
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <f>IF(ISBLANK(ui!I20),"",ui!I20)</f>
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <f>IF(ISBLANK(ui!J20),"",ui!J20)</f>
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <f>IF(ISBLANK(ui!K20),"",ui!K20)</f>
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <f>IF(ISBLANK(ui!L20),"",ui!L20)</f>
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <f>IF(ISBLANK(ui!M20),"",ui!M20)</f>
+        <v>3</v>
+      </c>
+      <c r="N6">
+        <f>IF(ISBLANK(ui!N20),"",ui!N20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
+        <f>IF(ISBLANK(ui!A21),"",ui!A21)</f>
+        <v/>
+      </c>
+      <c r="B7" t="str">
+        <f>IF(ISBLANK(ui!B21),"",ui!B21)</f>
+        <v/>
+      </c>
+      <c r="C7" t="str">
+        <f>IF(ISBLANK(ui!C21),"",ui!C21)</f>
+        <v/>
+      </c>
+      <c r="D7" t="str">
+        <f>IF(ISBLANK(ui!D21),"",ui!D21)</f>
+        <v/>
+      </c>
+      <c r="E7" t="str">
+        <f>IF(ISBLANK(ui!E21),"",ui!E21)</f>
+        <v/>
+      </c>
+      <c r="F7" t="str">
+        <f>IF(ISBLANK(ui!F21),"",ui!F21)</f>
+        <v/>
+      </c>
+      <c r="G7" t="str">
+        <f>IF(ISBLANK(ui!G21),"",ui!G21)</f>
+        <v/>
+      </c>
+      <c r="H7" t="str">
+        <f>IF(ISBLANK(ui!H21),"",ui!H21)</f>
+        <v/>
+      </c>
+      <c r="I7" t="str">
+        <f>IF(ISBLANK(ui!I21),"",ui!I21)</f>
+        <v/>
+      </c>
+      <c r="J7" t="str">
+        <f>IF(ISBLANK(ui!J21),"",ui!J21)</f>
+        <v/>
+      </c>
+      <c r="K7" t="str">
+        <f>IF(ISBLANK(ui!K21),"",ui!K21)</f>
+        <v/>
+      </c>
+      <c r="L7" t="str">
+        <f>IF(ISBLANK(ui!L21),"",ui!L21)</f>
+        <v/>
+      </c>
+      <c r="M7" t="str">
+        <f>IF(ISBLANK(ui!M21),"",ui!M21)</f>
+        <v/>
+      </c>
+      <c r="N7" t="str">
+        <f>IF(ISBLANK(ui!N21),"",ui!N21)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="str">
+        <f>IF(ISBLANK(ui!A22),"",ui!A22)</f>
+        <v/>
+      </c>
+      <c r="B8" t="str">
+        <f>IF(ISBLANK(ui!B22),"",ui!B22)</f>
+        <v/>
+      </c>
+      <c r="C8" t="str">
+        <f>IF(ISBLANK(ui!C22),"",ui!C22)</f>
+        <v/>
+      </c>
+      <c r="D8" t="str">
+        <f>IF(ISBLANK(ui!D22),"",ui!D22)</f>
+        <v/>
+      </c>
+      <c r="E8" t="str">
+        <f>IF(ISBLANK(ui!E22),"",ui!E22)</f>
+        <v/>
+      </c>
+      <c r="F8" t="str">
+        <f>IF(ISBLANK(ui!F22),"",ui!F22)</f>
+        <v/>
+      </c>
+      <c r="G8" t="str">
+        <f>IF(ISBLANK(ui!G22),"",ui!G22)</f>
+        <v/>
+      </c>
+      <c r="H8" t="str">
+        <f>IF(ISBLANK(ui!H22),"",ui!H22)</f>
+        <v/>
+      </c>
+      <c r="I8" t="str">
+        <f>IF(ISBLANK(ui!I22),"",ui!I22)</f>
+        <v/>
+      </c>
+      <c r="J8" t="str">
+        <f>IF(ISBLANK(ui!J22),"",ui!J22)</f>
+        <v/>
+      </c>
+      <c r="K8" t="str">
+        <f>IF(ISBLANK(ui!K22),"",ui!K22)</f>
+        <v/>
+      </c>
+      <c r="L8" t="str">
+        <f>IF(ISBLANK(ui!L22),"",ui!L22)</f>
+        <v/>
+      </c>
+      <c r="M8" t="str">
+        <f>IF(ISBLANK(ui!M22),"",ui!M22)</f>
+        <v/>
+      </c>
+      <c r="N8" t="str">
+        <f>IF(ISBLANK(ui!N22),"",ui!N22)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="str">
+        <f>IF(ISBLANK(ui!A23),"",ui!A23)</f>
+        <v/>
+      </c>
+      <c r="B9" t="str">
+        <f>IF(ISBLANK(ui!B23),"",ui!B23)</f>
+        <v/>
+      </c>
+      <c r="C9" t="str">
+        <f>IF(ISBLANK(ui!C23),"",ui!C23)</f>
+        <v/>
+      </c>
+      <c r="D9" t="str">
+        <f>IF(ISBLANK(ui!D23),"",ui!D23)</f>
+        <v/>
+      </c>
+      <c r="E9" t="str">
+        <f>IF(ISBLANK(ui!E23),"",ui!E23)</f>
+        <v/>
+      </c>
+      <c r="F9" t="str">
+        <f>IF(ISBLANK(ui!F23),"",ui!F23)</f>
+        <v/>
+      </c>
+      <c r="G9" t="str">
+        <f>IF(ISBLANK(ui!G23),"",ui!G23)</f>
+        <v/>
+      </c>
+      <c r="H9" t="str">
+        <f>IF(ISBLANK(ui!H23),"",ui!H23)</f>
+        <v/>
+      </c>
+      <c r="I9" t="str">
+        <f>IF(ISBLANK(ui!I23),"",ui!I23)</f>
+        <v/>
+      </c>
+      <c r="J9" t="str">
+        <f>IF(ISBLANK(ui!J23),"",ui!J23)</f>
+        <v/>
+      </c>
+      <c r="K9" t="str">
+        <f>IF(ISBLANK(ui!K23),"",ui!K23)</f>
+        <v/>
+      </c>
+      <c r="L9" t="str">
+        <f>IF(ISBLANK(ui!L23),"",ui!L23)</f>
+        <v/>
+      </c>
+      <c r="M9" t="str">
+        <f>IF(ISBLANK(ui!M23),"",ui!M23)</f>
+        <v/>
+      </c>
+      <c r="N9" t="str">
+        <f>IF(ISBLANK(ui!N23),"",ui!N23)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" t="str">
+        <f>IF(ISBLANK(ui!A24),"",ui!A24)</f>
+        <v/>
+      </c>
+      <c r="B10" t="str">
+        <f>IF(ISBLANK(ui!B24),"",ui!B24)</f>
+        <v/>
+      </c>
+      <c r="C10" t="str">
+        <f>IF(ISBLANK(ui!C24),"",ui!C24)</f>
+        <v/>
+      </c>
+      <c r="D10" t="str">
+        <f>IF(ISBLANK(ui!D24),"",ui!D24)</f>
+        <v/>
+      </c>
+      <c r="E10" t="str">
+        <f>IF(ISBLANK(ui!E24),"",ui!E24)</f>
+        <v/>
+      </c>
+      <c r="F10" t="str">
+        <f>IF(ISBLANK(ui!F24),"",ui!F24)</f>
+        <v/>
+      </c>
+      <c r="G10" t="str">
+        <f>IF(ISBLANK(ui!G24),"",ui!G24)</f>
+        <v/>
+      </c>
+      <c r="H10" t="str">
+        <f>IF(ISBLANK(ui!H24),"",ui!H24)</f>
+        <v/>
+      </c>
+      <c r="I10" t="str">
+        <f>IF(ISBLANK(ui!I24),"",ui!I24)</f>
+        <v/>
+      </c>
+      <c r="J10" t="str">
+        <f>IF(ISBLANK(ui!J24),"",ui!J24)</f>
+        <v/>
+      </c>
+      <c r="K10" t="str">
+        <f>IF(ISBLANK(ui!K24),"",ui!K24)</f>
+        <v/>
+      </c>
+      <c r="L10" t="str">
+        <f>IF(ISBLANK(ui!L24),"",ui!L24)</f>
+        <v/>
+      </c>
+      <c r="M10" t="str">
+        <f>IF(ISBLANK(ui!M24),"",ui!M24)</f>
+        <v/>
+      </c>
+      <c r="N10" t="str">
+        <f>IF(ISBLANK(ui!N24),"",ui!N24)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" t="str">
+        <f>IF(ISBLANK(ui!A25),"",ui!A25)</f>
+        <v/>
+      </c>
+      <c r="B11" t="str">
+        <f>IF(ISBLANK(ui!B25),"",ui!B25)</f>
+        <v/>
+      </c>
+      <c r="C11" t="str">
+        <f>IF(ISBLANK(ui!C25),"",ui!C25)</f>
+        <v/>
+      </c>
+      <c r="D11" t="str">
+        <f>IF(ISBLANK(ui!D25),"",ui!D25)</f>
+        <v/>
+      </c>
+      <c r="E11" t="str">
+        <f>IF(ISBLANK(ui!E25),"",ui!E25)</f>
+        <v/>
+      </c>
+      <c r="F11" t="str">
+        <f>IF(ISBLANK(ui!F25),"",ui!F25)</f>
+        <v/>
+      </c>
+      <c r="G11" t="str">
+        <f>IF(ISBLANK(ui!G25),"",ui!G25)</f>
+        <v/>
+      </c>
+      <c r="H11" t="str">
+        <f>IF(ISBLANK(ui!H25),"",ui!H25)</f>
+        <v/>
+      </c>
+      <c r="I11" t="str">
+        <f>IF(ISBLANK(ui!I25),"",ui!I25)</f>
+        <v/>
+      </c>
+      <c r="J11" t="str">
+        <f>IF(ISBLANK(ui!J25),"",ui!J25)</f>
+        <v/>
+      </c>
+      <c r="K11" t="str">
+        <f>IF(ISBLANK(ui!K25),"",ui!K25)</f>
+        <v/>
+      </c>
+      <c r="L11" t="str">
+        <f>IF(ISBLANK(ui!L25),"",ui!L25)</f>
+        <v/>
+      </c>
+      <c r="M11" t="str">
+        <f>IF(ISBLANK(ui!M25),"",ui!M25)</f>
+        <v/>
+      </c>
+      <c r="N11" t="str">
+        <f>IF(ISBLANK(ui!N25),"",ui!N25)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
+        <f>IF(ISBLANK(ui!A26),"",ui!A26)</f>
+        <v/>
+      </c>
+      <c r="B12" t="str">
+        <f>IF(ISBLANK(ui!B26),"",ui!B26)</f>
+        <v/>
+      </c>
+      <c r="C12" t="str">
+        <f>IF(ISBLANK(ui!C26),"",ui!C26)</f>
+        <v/>
+      </c>
+      <c r="D12" t="str">
+        <f>IF(ISBLANK(ui!D26),"",ui!D26)</f>
+        <v/>
+      </c>
+      <c r="E12" t="str">
+        <f>IF(ISBLANK(ui!E26),"",ui!E26)</f>
+        <v/>
+      </c>
+      <c r="F12" t="str">
+        <f>IF(ISBLANK(ui!F26),"",ui!F26)</f>
+        <v/>
+      </c>
+      <c r="G12" t="str">
+        <f>IF(ISBLANK(ui!G26),"",ui!G26)</f>
+        <v/>
+      </c>
+      <c r="H12" t="str">
+        <f>IF(ISBLANK(ui!H26),"",ui!H26)</f>
+        <v/>
+      </c>
+      <c r="I12" t="str">
+        <f>IF(ISBLANK(ui!I26),"",ui!I26)</f>
+        <v/>
+      </c>
+      <c r="J12" t="str">
+        <f>IF(ISBLANK(ui!J26),"",ui!J26)</f>
+        <v/>
+      </c>
+      <c r="K12" t="str">
+        <f>IF(ISBLANK(ui!K26),"",ui!K26)</f>
+        <v/>
+      </c>
+      <c r="L12" t="str">
+        <f>IF(ISBLANK(ui!L26),"",ui!L26)</f>
+        <v/>
+      </c>
+      <c r="M12" t="str">
+        <f>IF(ISBLANK(ui!M26),"",ui!M26)</f>
+        <v/>
+      </c>
+      <c r="N12" t="str">
+        <f>IF(ISBLANK(ui!N26),"",ui!N26)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" t="str">
+        <f>IF(ISBLANK(ui!A27),"",ui!A27)</f>
+        <v/>
+      </c>
+      <c r="B13" t="str">
+        <f>IF(ISBLANK(ui!B27),"",ui!B27)</f>
+        <v/>
+      </c>
+      <c r="C13" t="str">
+        <f>IF(ISBLANK(ui!C27),"",ui!C27)</f>
+        <v/>
+      </c>
+      <c r="D13" t="str">
+        <f>IF(ISBLANK(ui!D27),"",ui!D27)</f>
+        <v/>
+      </c>
+      <c r="E13" t="str">
+        <f>IF(ISBLANK(ui!E27),"",ui!E27)</f>
+        <v/>
+      </c>
+      <c r="F13" t="str">
+        <f>IF(ISBLANK(ui!F27),"",ui!F27)</f>
+        <v/>
+      </c>
+      <c r="G13" t="str">
+        <f>IF(ISBLANK(ui!G27),"",ui!G27)</f>
+        <v/>
+      </c>
+      <c r="H13" t="str">
+        <f>IF(ISBLANK(ui!H27),"",ui!H27)</f>
+        <v/>
+      </c>
+      <c r="I13" t="str">
+        <f>IF(ISBLANK(ui!I27),"",ui!I27)</f>
+        <v/>
+      </c>
+      <c r="J13" t="str">
+        <f>IF(ISBLANK(ui!J27),"",ui!J27)</f>
+        <v/>
+      </c>
+      <c r="K13" t="str">
+        <f>IF(ISBLANK(ui!K27),"",ui!K27)</f>
+        <v/>
+      </c>
+      <c r="L13" t="str">
+        <f>IF(ISBLANK(ui!L27),"",ui!L27)</f>
+        <v/>
+      </c>
+      <c r="M13" t="str">
+        <f>IF(ISBLANK(ui!M27),"",ui!M27)</f>
+        <v/>
+      </c>
+      <c r="N13" t="str">
+        <f>IF(ISBLANK(ui!N27),"",ui!N27)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" t="str">
+        <f>IF(ISBLANK(ui!A28),"",ui!A28)</f>
+        <v/>
+      </c>
+      <c r="B14" t="str">
+        <f>IF(ISBLANK(ui!B28),"",ui!B28)</f>
+        <v/>
+      </c>
+      <c r="C14" t="str">
+        <f>IF(ISBLANK(ui!C28),"",ui!C28)</f>
+        <v/>
+      </c>
+      <c r="D14" t="str">
+        <f>IF(ISBLANK(ui!D28),"",ui!D28)</f>
+        <v/>
+      </c>
+      <c r="E14" t="str">
+        <f>IF(ISBLANK(ui!E28),"",ui!E28)</f>
+        <v/>
+      </c>
+      <c r="F14" t="str">
+        <f>IF(ISBLANK(ui!F28),"",ui!F28)</f>
+        <v/>
+      </c>
+      <c r="G14" t="str">
+        <f>IF(ISBLANK(ui!G28),"",ui!G28)</f>
+        <v/>
+      </c>
+      <c r="H14" t="str">
+        <f>IF(ISBLANK(ui!H28),"",ui!H28)</f>
+        <v/>
+      </c>
+      <c r="I14" t="str">
+        <f>IF(ISBLANK(ui!I28),"",ui!I28)</f>
+        <v/>
+      </c>
+      <c r="J14" t="str">
+        <f>IF(ISBLANK(ui!J28),"",ui!J28)</f>
+        <v/>
+      </c>
+      <c r="K14" t="str">
+        <f>IF(ISBLANK(ui!K28),"",ui!K28)</f>
+        <v/>
+      </c>
+      <c r="L14" t="str">
+        <f>IF(ISBLANK(ui!L28),"",ui!L28)</f>
+        <v/>
+      </c>
+      <c r="M14" t="str">
+        <f>IF(ISBLANK(ui!M28),"",ui!M28)</f>
+        <v/>
+      </c>
+      <c r="N14" t="str">
+        <f>IF(ISBLANK(ui!N28),"",ui!N28)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" t="str">
+        <f>IF(ISBLANK(ui!A29),"",ui!A29)</f>
+        <v/>
+      </c>
+      <c r="B15" t="str">
+        <f>IF(ISBLANK(ui!B29),"",ui!B29)</f>
+        <v/>
+      </c>
+      <c r="C15" t="str">
+        <f>IF(ISBLANK(ui!C29),"",ui!C29)</f>
+        <v/>
+      </c>
+      <c r="D15" t="str">
+        <f>IF(ISBLANK(ui!D29),"",ui!D29)</f>
+        <v/>
+      </c>
+      <c r="E15" t="str">
+        <f>IF(ISBLANK(ui!E29),"",ui!E29)</f>
+        <v/>
+      </c>
+      <c r="F15" t="str">
+        <f>IF(ISBLANK(ui!F29),"",ui!F29)</f>
+        <v/>
+      </c>
+      <c r="G15" t="str">
+        <f>IF(ISBLANK(ui!G29),"",ui!G29)</f>
+        <v/>
+      </c>
+      <c r="H15" t="str">
+        <f>IF(ISBLANK(ui!H29),"",ui!H29)</f>
+        <v/>
+      </c>
+      <c r="I15" t="str">
+        <f>IF(ISBLANK(ui!I29),"",ui!I29)</f>
+        <v/>
+      </c>
+      <c r="J15" t="str">
+        <f>IF(ISBLANK(ui!J29),"",ui!J29)</f>
+        <v/>
+      </c>
+      <c r="K15" t="str">
+        <f>IF(ISBLANK(ui!K29),"",ui!K29)</f>
+        <v/>
+      </c>
+      <c r="L15" t="str">
+        <f>IF(ISBLANK(ui!L29),"",ui!L29)</f>
+        <v/>
+      </c>
+      <c r="M15" t="str">
+        <f>IF(ISBLANK(ui!M29),"",ui!M29)</f>
+        <v/>
+      </c>
+      <c r="N15" t="str">
+        <f>IF(ISBLANK(ui!N29),"",ui!N29)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" t="str">
+        <f>IF(ISBLANK(ui!A30),"",ui!A30)</f>
+        <v/>
+      </c>
+      <c r="B16" t="str">
+        <f>IF(ISBLANK(ui!B30),"",ui!B30)</f>
+        <v/>
+      </c>
+      <c r="C16" t="str">
+        <f>IF(ISBLANK(ui!C30),"",ui!C30)</f>
+        <v/>
+      </c>
+      <c r="D16" t="str">
+        <f>IF(ISBLANK(ui!D30),"",ui!D30)</f>
+        <v/>
+      </c>
+      <c r="E16" t="str">
+        <f>IF(ISBLANK(ui!E30),"",ui!E30)</f>
+        <v/>
+      </c>
+      <c r="F16" t="str">
+        <f>IF(ISBLANK(ui!F30),"",ui!F30)</f>
+        <v/>
+      </c>
+      <c r="G16" t="str">
+        <f>IF(ISBLANK(ui!G30),"",ui!G30)</f>
+        <v/>
+      </c>
+      <c r="H16" t="str">
+        <f>IF(ISBLANK(ui!H30),"",ui!H30)</f>
+        <v/>
+      </c>
+      <c r="I16" t="str">
+        <f>IF(ISBLANK(ui!I30),"",ui!I30)</f>
+        <v/>
+      </c>
+      <c r="J16" t="str">
+        <f>IF(ISBLANK(ui!J30),"",ui!J30)</f>
+        <v/>
+      </c>
+      <c r="K16" t="str">
+        <f>IF(ISBLANK(ui!K30),"",ui!K30)</f>
+        <v/>
+      </c>
+      <c r="L16" t="str">
+        <f>IF(ISBLANK(ui!L30),"",ui!L30)</f>
+        <v/>
+      </c>
+      <c r="M16" t="str">
+        <f>IF(ISBLANK(ui!M30),"",ui!M30)</f>
+        <v/>
+      </c>
+      <c r="N16" t="str">
+        <f>IF(ISBLANK(ui!N30),"",ui!N30)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" t="str">
+        <f>IF(ISBLANK(ui!A31),"",ui!A31)</f>
+        <v/>
+      </c>
+      <c r="B17" t="str">
+        <f>IF(ISBLANK(ui!B31),"",ui!B31)</f>
+        <v/>
+      </c>
+      <c r="C17" t="str">
+        <f>IF(ISBLANK(ui!C31),"",ui!C31)</f>
+        <v/>
+      </c>
+      <c r="D17" t="str">
+        <f>IF(ISBLANK(ui!D31),"",ui!D31)</f>
+        <v/>
+      </c>
+      <c r="E17" t="str">
+        <f>IF(ISBLANK(ui!E31),"",ui!E31)</f>
+        <v/>
+      </c>
+      <c r="F17" t="str">
+        <f>IF(ISBLANK(ui!F31),"",ui!F31)</f>
+        <v/>
+      </c>
+      <c r="G17" t="str">
+        <f>IF(ISBLANK(ui!G31),"",ui!G31)</f>
+        <v/>
+      </c>
+      <c r="H17" t="str">
+        <f>IF(ISBLANK(ui!H31),"",ui!H31)</f>
+        <v/>
+      </c>
+      <c r="I17" t="str">
+        <f>IF(ISBLANK(ui!I31),"",ui!I31)</f>
+        <v/>
+      </c>
+      <c r="J17" t="str">
+        <f>IF(ISBLANK(ui!J31),"",ui!J31)</f>
+        <v/>
+      </c>
+      <c r="K17" t="str">
+        <f>IF(ISBLANK(ui!K31),"",ui!K31)</f>
+        <v/>
+      </c>
+      <c r="L17" t="str">
+        <f>IF(ISBLANK(ui!L31),"",ui!L31)</f>
+        <v/>
+      </c>
+      <c r="M17" t="str">
+        <f>IF(ISBLANK(ui!M31),"",ui!M31)</f>
+        <v/>
+      </c>
+      <c r="N17" t="str">
+        <f>IF(ISBLANK(ui!N31),"",ui!N31)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" t="str">
+        <f>IF(ISBLANK(ui!A32),"",ui!A32)</f>
+        <v/>
+      </c>
+      <c r="B18" t="str">
+        <f>IF(ISBLANK(ui!B32),"",ui!B32)</f>
+        <v/>
+      </c>
+      <c r="C18" t="str">
+        <f>IF(ISBLANK(ui!C32),"",ui!C32)</f>
+        <v/>
+      </c>
+      <c r="D18" t="str">
+        <f>IF(ISBLANK(ui!D32),"",ui!D32)</f>
+        <v/>
+      </c>
+      <c r="E18" t="str">
+        <f>IF(ISBLANK(ui!E32),"",ui!E32)</f>
+        <v/>
+      </c>
+      <c r="F18" t="str">
+        <f>IF(ISBLANK(ui!F32),"",ui!F32)</f>
+        <v/>
+      </c>
+      <c r="G18" t="str">
+        <f>IF(ISBLANK(ui!G32),"",ui!G32)</f>
+        <v/>
+      </c>
+      <c r="H18" t="str">
+        <f>IF(ISBLANK(ui!H32),"",ui!H32)</f>
+        <v/>
+      </c>
+      <c r="I18" t="str">
+        <f>IF(ISBLANK(ui!I32),"",ui!I32)</f>
+        <v/>
+      </c>
+      <c r="J18" t="str">
+        <f>IF(ISBLANK(ui!J32),"",ui!J32)</f>
+        <v/>
+      </c>
+      <c r="K18" t="str">
+        <f>IF(ISBLANK(ui!K32),"",ui!K32)</f>
+        <v/>
+      </c>
+      <c r="L18" t="str">
+        <f>IF(ISBLANK(ui!L32),"",ui!L32)</f>
+        <v/>
+      </c>
+      <c r="M18" t="str">
+        <f>IF(ISBLANK(ui!M32),"",ui!M32)</f>
+        <v/>
+      </c>
+      <c r="N18" t="str">
+        <f>IF(ISBLANK(ui!N32),"",ui!N32)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" t="str">
+        <f>IF(ISBLANK(ui!A33),"",ui!A33)</f>
+        <v/>
+      </c>
+      <c r="B19" t="str">
+        <f>IF(ISBLANK(ui!B33),"",ui!B33)</f>
+        <v/>
+      </c>
+      <c r="C19" t="str">
+        <f>IF(ISBLANK(ui!C33),"",ui!C33)</f>
+        <v/>
+      </c>
+      <c r="D19" t="str">
+        <f>IF(ISBLANK(ui!D33),"",ui!D33)</f>
+        <v/>
+      </c>
+      <c r="E19" t="str">
+        <f>IF(ISBLANK(ui!E33),"",ui!E33)</f>
+        <v/>
+      </c>
+      <c r="F19" t="str">
+        <f>IF(ISBLANK(ui!F33),"",ui!F33)</f>
+        <v/>
+      </c>
+      <c r="G19" t="str">
+        <f>IF(ISBLANK(ui!G33),"",ui!G33)</f>
+        <v/>
+      </c>
+      <c r="H19" t="str">
+        <f>IF(ISBLANK(ui!H33),"",ui!H33)</f>
+        <v/>
+      </c>
+      <c r="I19" t="str">
+        <f>IF(ISBLANK(ui!I33),"",ui!I33)</f>
+        <v/>
+      </c>
+      <c r="J19" t="str">
+        <f>IF(ISBLANK(ui!J33),"",ui!J33)</f>
+        <v/>
+      </c>
+      <c r="K19" t="str">
+        <f>IF(ISBLANK(ui!K33),"",ui!K33)</f>
+        <v/>
+      </c>
+      <c r="L19" t="str">
+        <f>IF(ISBLANK(ui!L33),"",ui!L33)</f>
+        <v/>
+      </c>
+      <c r="M19" t="str">
+        <f>IF(ISBLANK(ui!M33),"",ui!M33)</f>
+        <v/>
+      </c>
+      <c r="N19" t="str">
+        <f>IF(ISBLANK(ui!N33),"",ui!N33)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" t="str">
+        <f>IF(ISBLANK(ui!A34),"",ui!A34)</f>
+        <v/>
+      </c>
+      <c r="B20" t="str">
+        <f>IF(ISBLANK(ui!B34),"",ui!B34)</f>
+        <v/>
+      </c>
+      <c r="C20" t="str">
+        <f>IF(ISBLANK(ui!C34),"",ui!C34)</f>
+        <v/>
+      </c>
+      <c r="D20" t="str">
+        <f>IF(ISBLANK(ui!D34),"",ui!D34)</f>
+        <v/>
+      </c>
+      <c r="E20" t="str">
+        <f>IF(ISBLANK(ui!E34),"",ui!E34)</f>
+        <v/>
+      </c>
+      <c r="F20" t="str">
+        <f>IF(ISBLANK(ui!F34),"",ui!F34)</f>
+        <v/>
+      </c>
+      <c r="G20" t="str">
+        <f>IF(ISBLANK(ui!G34),"",ui!G34)</f>
+        <v/>
+      </c>
+      <c r="H20" t="str">
+        <f>IF(ISBLANK(ui!H34),"",ui!H34)</f>
+        <v/>
+      </c>
+      <c r="I20" t="str">
+        <f>IF(ISBLANK(ui!I34),"",ui!I34)</f>
+        <v/>
+      </c>
+      <c r="J20" t="str">
+        <f>IF(ISBLANK(ui!J34),"",ui!J34)</f>
+        <v/>
+      </c>
+      <c r="K20" t="str">
+        <f>IF(ISBLANK(ui!K34),"",ui!K34)</f>
+        <v/>
+      </c>
+      <c r="L20" t="str">
+        <f>IF(ISBLANK(ui!L34),"",ui!L34)</f>
+        <v/>
+      </c>
+      <c r="M20" t="str">
+        <f>IF(ISBLANK(ui!M34),"",ui!M34)</f>
+        <v/>
+      </c>
+      <c r="N20" t="str">
+        <f>IF(ISBLANK(ui!N34),"",ui!N34)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" t="str">
+        <f>IF(ISBLANK(ui!A35),"",ui!A35)</f>
+        <v/>
+      </c>
+      <c r="B21" t="str">
+        <f>IF(ISBLANK(ui!B35),"",ui!B35)</f>
+        <v/>
+      </c>
+      <c r="C21" t="str">
+        <f>IF(ISBLANK(ui!C35),"",ui!C35)</f>
+        <v/>
+      </c>
+      <c r="D21" t="str">
+        <f>IF(ISBLANK(ui!D35),"",ui!D35)</f>
+        <v/>
+      </c>
+      <c r="E21" t="str">
+        <f>IF(ISBLANK(ui!E35),"",ui!E35)</f>
+        <v/>
+      </c>
+      <c r="F21" t="str">
+        <f>IF(ISBLANK(ui!F35),"",ui!F35)</f>
+        <v/>
+      </c>
+      <c r="G21" t="str">
+        <f>IF(ISBLANK(ui!G35),"",ui!G35)</f>
+        <v/>
+      </c>
+      <c r="H21" t="str">
+        <f>IF(ISBLANK(ui!H35),"",ui!H35)</f>
+        <v/>
+      </c>
+      <c r="I21" t="str">
+        <f>IF(ISBLANK(ui!I35),"",ui!I35)</f>
+        <v/>
+      </c>
+      <c r="J21" t="str">
+        <f>IF(ISBLANK(ui!J35),"",ui!J35)</f>
+        <v/>
+      </c>
+      <c r="K21" t="str">
+        <f>IF(ISBLANK(ui!K35),"",ui!K35)</f>
+        <v/>
+      </c>
+      <c r="L21" t="str">
+        <f>IF(ISBLANK(ui!L35),"",ui!L35)</f>
+        <v/>
+      </c>
+      <c r="M21" t="str">
+        <f>IF(ISBLANK(ui!M35),"",ui!M35)</f>
+        <v/>
+      </c>
+      <c r="N21" t="str">
+        <f>IF(ISBLANK(ui!N35),"",ui!N35)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" t="str">
+        <f>IF(ISBLANK(ui!A36),"",ui!A36)</f>
+        <v/>
+      </c>
+      <c r="B22" t="str">
+        <f>IF(ISBLANK(ui!B36),"",ui!B36)</f>
+        <v/>
+      </c>
+      <c r="C22" t="str">
+        <f>IF(ISBLANK(ui!C36),"",ui!C36)</f>
+        <v/>
+      </c>
+      <c r="D22" t="str">
+        <f>IF(ISBLANK(ui!D36),"",ui!D36)</f>
+        <v/>
+      </c>
+      <c r="E22" t="str">
+        <f>IF(ISBLANK(ui!E36),"",ui!E36)</f>
+        <v/>
+      </c>
+      <c r="F22" t="str">
+        <f>IF(ISBLANK(ui!F36),"",ui!F36)</f>
+        <v/>
+      </c>
+      <c r="G22" t="str">
+        <f>IF(ISBLANK(ui!G36),"",ui!G36)</f>
+        <v/>
+      </c>
+      <c r="H22" t="str">
+        <f>IF(ISBLANK(ui!H36),"",ui!H36)</f>
+        <v/>
+      </c>
+      <c r="I22" t="str">
+        <f>IF(ISBLANK(ui!I36),"",ui!I36)</f>
+        <v/>
+      </c>
+      <c r="J22" t="str">
+        <f>IF(ISBLANK(ui!J36),"",ui!J36)</f>
+        <v/>
+      </c>
+      <c r="K22" t="str">
+        <f>IF(ISBLANK(ui!K36),"",ui!K36)</f>
+        <v/>
+      </c>
+      <c r="L22" t="str">
+        <f>IF(ISBLANK(ui!L36),"",ui!L36)</f>
+        <v/>
+      </c>
+      <c r="M22" t="str">
+        <f>IF(ISBLANK(ui!M36),"",ui!M36)</f>
+        <v/>
+      </c>
+      <c r="N22" t="str">
+        <f>IF(ISBLANK(ui!N36),"",ui!N36)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" t="str">
+        <f>IF(ISBLANK(ui!A37),"",ui!A37)</f>
+        <v/>
+      </c>
+      <c r="B23" t="str">
+        <f>IF(ISBLANK(ui!B37),"",ui!B37)</f>
+        <v/>
+      </c>
+      <c r="C23" t="str">
+        <f>IF(ISBLANK(ui!C37),"",ui!C37)</f>
+        <v/>
+      </c>
+      <c r="D23" t="str">
+        <f>IF(ISBLANK(ui!D37),"",ui!D37)</f>
+        <v/>
+      </c>
+      <c r="E23" t="str">
+        <f>IF(ISBLANK(ui!E37),"",ui!E37)</f>
+        <v/>
+      </c>
+      <c r="F23" t="str">
+        <f>IF(ISBLANK(ui!F37),"",ui!F37)</f>
+        <v/>
+      </c>
+      <c r="G23" t="str">
+        <f>IF(ISBLANK(ui!G37),"",ui!G37)</f>
+        <v/>
+      </c>
+      <c r="H23" t="str">
+        <f>IF(ISBLANK(ui!H37),"",ui!H37)</f>
+        <v/>
+      </c>
+      <c r="I23" t="str">
+        <f>IF(ISBLANK(ui!I37),"",ui!I37)</f>
+        <v/>
+      </c>
+      <c r="J23" t="str">
+        <f>IF(ISBLANK(ui!J37),"",ui!J37)</f>
+        <v/>
+      </c>
+      <c r="K23" t="str">
+        <f>IF(ISBLANK(ui!K37),"",ui!K37)</f>
+        <v/>
+      </c>
+      <c r="L23" t="str">
+        <f>IF(ISBLANK(ui!L37),"",ui!L37)</f>
+        <v/>
+      </c>
+      <c r="M23" t="str">
+        <f>IF(ISBLANK(ui!M37),"",ui!M37)</f>
+        <v/>
+      </c>
+      <c r="N23" t="str">
+        <f>IF(ISBLANK(ui!N37),"",ui!N37)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE578704-8EA0-4F61-A644-20F07D719928}">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
@@ -6885,12 +8235,12 @@
       <c r="F1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="G1" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
       <c r="K1" s="1" t="s">
         <v>109</v>
       </c>

</xml_diff>

<commit_message>
automatic tilemap to excel
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E9D790-4410-41BB-9434-3CD42876B00F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064384DC-D3C7-4109-9501-07B74EE27091}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ui" sheetId="10" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="120">
   <si>
     <t>id</t>
   </si>
@@ -187,9 +187,6 @@
     <t>well</t>
   </si>
   <si>
-    <t>farmacy</t>
-  </si>
-  <si>
     <t>workshop</t>
   </si>
   <si>
@@ -449,6 +446,12 @@
   </si>
   <si>
     <t>count</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>pharmacy</t>
   </si>
 </sst>
 </file>
@@ -847,8 +850,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>Tile type distribution</a:t>
+              <a:t>Tile</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" baseline="0"/>
+              <a:t> types</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1218,6 +1226,412 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Resource production</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-2CB7-4215-A448-9AF1989B785B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-2CB7-4215-A448-9AF1989B785B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-2CB7-4215-A448-9AF1989B785B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-2CB7-4215-A448-9AF1989B785B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-2CB7-4215-A448-9AF1989B785B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-2CB7-4215-A448-9AF1989B785B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-2CB7-4215-A448-9AF1989B785B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-2CB7-4215-A448-9AF1989B785B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>s_map_tiles!$I$1:$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>water</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>food</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>medicines</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>rock</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>wood</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tools</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>weapons</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>information</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>s_map_tiles!$I$10:$P$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>394</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000010-2CB7-4215-A448-9AF1989B785B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1258,7 +1672,566 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3058,13 +4031,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3089,6 +4062,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>302895</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>36195</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D898E698-9D06-4B30-BD78-3C8A41C96594}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3373,406 +4384,406 @@
   <sheetData>
     <row r="1" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="F1" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="50" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="G1" s="50" t="s">
-        <v>62</v>
-      </c>
       <c r="H1" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I1" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J1" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K1" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L1" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M1" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N1" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O1" s="11"/>
     </row>
     <row r="2" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D2" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E2" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="G2" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="H2" s="50" t="s">
-        <v>62</v>
-      </c>
       <c r="I2" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J2" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K2" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L2" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M2" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N2" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O2" s="11"/>
     </row>
     <row r="3" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E3" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="F3" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="H3" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="I3" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="J3" s="50" t="s">
-        <v>62</v>
-      </c>
       <c r="K3" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L3" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M3" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N3" s="51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O3" s="11"/>
     </row>
     <row r="4" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F4" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="L4" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="M4" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="H4" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="I4" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="J4" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="K4" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="L4" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="M4" s="50" t="s">
-        <v>62</v>
-      </c>
       <c r="N4" s="51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O4" s="11"/>
     </row>
     <row r="5" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D5" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G5" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H5" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I5" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J5" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K5" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L5" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M5" s="50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N5" s="51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O5" s="11"/>
     </row>
     <row r="6" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G6" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H6" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I6" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J6" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K6" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L6" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M6" s="50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N6" s="51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O6" s="11"/>
     </row>
     <row r="7" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E7" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F7" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G7" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H7" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I7" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J7" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="K7" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="L7" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="K7" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="L7" s="50" t="s">
-        <v>62</v>
-      </c>
       <c r="M7" s="50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N7" s="51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O7" s="11"/>
     </row>
     <row r="8" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E8" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F8" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G8" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H8" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I8" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J8" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K8" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="L8" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="L8" s="50" t="s">
-        <v>62</v>
-      </c>
       <c r="M8" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="N8" s="51" t="s">
         <v>61</v>
-      </c>
-      <c r="N8" s="51" t="s">
-        <v>62</v>
       </c>
       <c r="O8" s="11"/>
     </row>
     <row r="9" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D9" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E9" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F9" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G9" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="J9" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="K9" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="L9" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="H9" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="I9" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="J9" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="K9" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="L9" s="50" t="s">
+      <c r="N9" s="51" t="s">
         <v>61</v>
-      </c>
-      <c r="M9" s="50" t="s">
-        <v>62</v>
-      </c>
-      <c r="N9" s="51" t="s">
-        <v>62</v>
       </c>
       <c r="O9" s="11"/>
       <c r="R9" s="12"/>
@@ -3780,219 +4791,219 @@
     </row>
     <row r="10" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E10" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F10" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G10" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H10" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I10" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J10" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K10" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L10" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M10" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N10" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O10" s="11"/>
       <c r="P10" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q10" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="Q10" s="40" t="s">
+      <c r="R10" s="41" t="s">
         <v>98</v>
-      </c>
-      <c r="R10" s="41" t="s">
-        <v>99</v>
       </c>
       <c r="V10" s="12"/>
     </row>
     <row r="11" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D11" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E11" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="50" t="s">
-        <v>62</v>
-      </c>
       <c r="G11" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="J11" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="K11" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="L11" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="I11" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="J11" s="50" t="s">
+      <c r="M11" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="N11" s="51" t="s">
         <v>61</v>
-      </c>
-      <c r="K11" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="L11" s="50" t="s">
-        <v>62</v>
-      </c>
-      <c r="M11" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="N11" s="51" t="s">
-        <v>62</v>
       </c>
       <c r="O11" s="11"/>
       <c r="P11" s="42">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q11" s="43">
         <f t="shared" ref="Q11:Q12" ca="1" si="0">RANDBETWEEN(1,6)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R11" s="44">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V11" s="12"/>
     </row>
     <row r="12" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D12" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E12" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F12" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G12" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="J12" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="I12" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="J12" s="50" t="s">
-        <v>62</v>
-      </c>
       <c r="K12" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L12" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M12" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N12" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O12" s="11"/>
       <c r="P12" s="42">
         <f t="shared" ref="P12:P14" ca="1" si="1">RANDBETWEEN(1,6)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q12" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R12" s="45"/>
       <c r="V12" s="12"/>
     </row>
     <row r="13" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E13" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F13" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="I13" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="K13" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="G13" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="H13" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="I13" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="J13" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="K13" s="50" t="s">
-        <v>62</v>
-      </c>
       <c r="L13" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M13" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N13" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O13" s="11"/>
       <c r="P13" s="42">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="Q13" s="46"/>
       <c r="R13" s="45"/>
@@ -4000,51 +5011,51 @@
     </row>
     <row r="14" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D14" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E14" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F14" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G14" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H14" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I14" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J14" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K14" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L14" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M14" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N14" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O14" s="11"/>
       <c r="P14" s="47">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q14" s="18"/>
       <c r="R14" s="48"/>
@@ -4061,7 +5072,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="54" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D15" s="52" t="s">
         <v>9</v>
@@ -4088,13 +5099,13 @@
         <v>24</v>
       </c>
       <c r="L15" s="52" t="s">
+        <v>104</v>
+      </c>
+      <c r="M15" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="M15" s="54" t="s">
+      <c r="N15" s="54" t="s">
         <v>106</v>
-      </c>
-      <c r="N15" s="54" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
@@ -4102,7 +5113,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C16" s="13">
         <v>3</v>
@@ -4146,7 +5157,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C17" s="13">
         <v>3</v>
@@ -4190,7 +5201,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C18" s="13">
         <v>3</v>
@@ -4234,7 +5245,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C19" s="13">
         <v>3</v>
@@ -4278,7 +5289,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C20" s="48">
         <v>3</v>
@@ -4644,16 +5655,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>29</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4670,10 +5681,10 @@
         <v>23</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
@@ -4690,7 +5701,7 @@
         <v>23</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F3" s="9"/>
     </row>
@@ -4705,13 +5716,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4728,7 +5739,7 @@
         <v>22</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F5" s="9"/>
     </row>
@@ -4746,7 +5757,7 @@
         <v>22</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F6" s="9"/>
     </row>
@@ -4764,10 +5775,10 @@
         <v>20</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4784,10 +5795,10 @@
         <v>21</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4804,10 +5815,10 @@
         <v>25</v>
       </c>
       <c r="E9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -4819,15 +5830,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5531790B-02F5-4EEF-93DC-68D09484BB8E}">
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D1" s="59" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E1" s="60"/>
       <c r="F1" s="60"/>
@@ -4836,7 +5847,7 @@
       <c r="I1" s="60"/>
       <c r="J1" s="12"/>
       <c r="K1" s="59" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L1" s="60"/>
       <c r="M1" s="60"/>
@@ -4854,7 +5865,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" s="28" t="s">
         <v>14</v>
@@ -4942,7 +5953,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -4978,7 +5989,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>119</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -5018,7 +6029,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -5048,14 +6059,14 @@
         <v>-1</v>
       </c>
       <c r="P6" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q6" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R6" s="13"/>
       <c r="T6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
@@ -5063,7 +6074,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -5099,7 +6110,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -5135,7 +6146,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
@@ -5166,7 +6177,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="12"/>
@@ -5199,7 +6210,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="12"/>
@@ -5230,7 +6241,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
@@ -5423,10 +6434,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -5437,14 +6448,14 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D2" s="33">
         <f t="shared" ref="D2:D7" si="0">B2/SUM(B:B)</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="E2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -5455,14 +6466,14 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3" s="33">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -5473,14 +6484,14 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4" s="33">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -5491,14 +6502,14 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" s="33">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -5509,14 +6520,14 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6" s="33">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
       <c r="E6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -5527,14 +6538,14 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D7" s="33">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -5566,10 +6577,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -5580,7 +6591,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D2" s="33">
         <f t="shared" ref="D2:D23" si="0">B2/SUM(B:B)</f>
@@ -5603,7 +6614,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D3" s="33">
         <f t="shared" si="0"/>
@@ -5622,7 +6633,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D4" s="33">
         <f t="shared" si="0"/>
@@ -5641,7 +6652,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D5" s="33">
         <f t="shared" si="0"/>
@@ -5660,7 +6671,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D6" s="33">
         <f t="shared" si="0"/>
@@ -5679,7 +6690,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D7" s="33">
         <f t="shared" si="0"/>
@@ -5698,7 +6709,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D8" s="33">
         <f t="shared" si="0"/>
@@ -5717,7 +6728,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D9" s="33">
         <f t="shared" si="0"/>
@@ -5736,14 +6747,14 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D10" s="33">
         <f t="shared" si="0"/>
         <v>6.4220183486238536E-2</v>
       </c>
       <c r="E10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
@@ -5754,14 +6765,14 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D11" s="33">
         <f t="shared" si="0"/>
         <v>2.7522935779816515E-2</v>
       </c>
       <c r="E11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
@@ -5772,14 +6783,14 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D12" s="33">
         <f t="shared" si="0"/>
         <v>0.13761467889908258</v>
       </c>
       <c r="E12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -5790,14 +6801,14 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D13" s="33">
         <f t="shared" si="0"/>
         <v>0.11009174311926606</v>
       </c>
       <c r="E13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
@@ -5808,7 +6819,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D14" s="33">
         <f t="shared" si="0"/>
@@ -5827,7 +6838,7 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D15" s="33">
         <f t="shared" si="0"/>
@@ -5846,7 +6857,7 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D16" s="33">
         <f t="shared" si="0"/>
@@ -5854,7 +6865,7 @@
       </c>
       <c r="E16" t="str">
         <f>_xlfn.CONCAT(_xlfn.CONCAT("You found a ",UPPER(buildings!B5)),"! Place it in whichever building (not necessarily yours) or tile you want")</f>
-        <v>You found a FARMACY! Place it in whichever building (not necessarily yours) or tile you want</v>
+        <v>You found a PHARMACY! Place it in whichever building (not necessarily yours) or tile you want</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
@@ -5865,7 +6876,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D17" s="33">
         <f t="shared" si="0"/>
@@ -5884,7 +6895,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D18" s="33">
         <f t="shared" si="0"/>
@@ -5903,7 +6914,7 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D19" s="33">
         <f t="shared" si="0"/>
@@ -5923,7 +6934,7 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D20" s="33">
         <f t="shared" si="0"/>
@@ -5942,7 +6953,7 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D21" s="33">
         <f t="shared" si="0"/>
@@ -5961,7 +6972,7 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D22" s="33">
         <f t="shared" si="0"/>
@@ -5980,7 +6991,7 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D23" s="33">
         <f t="shared" si="0"/>
@@ -6022,10 +7033,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="56" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D1" s="56" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -6033,13 +7044,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C2" s="55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" s="55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -6050,10 +7061,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="55" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D3" s="55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -6064,10 +7075,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D4" s="55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -6078,10 +7089,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" s="55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -6092,10 +7103,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" s="55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -6106,10 +7117,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="55" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D7" s="55" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -6120,10 +7131,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" s="55" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -6134,10 +7145,10 @@
         <v>11</v>
       </c>
       <c r="C9" s="55" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -7496,18 +8507,18 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DF0812B-FD6E-4752-AC5F-F1FB101103C6}">
-  <dimension ref="A1:U11"/>
+  <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="15" width="5.6640625" customWidth="1"/>
+    <col min="4" max="16" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="4" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="4" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -7515,7 +8526,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>12</v>
@@ -7533,35 +8544,38 @@
         <v>26</v>
       </c>
       <c r="I1" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="K1" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="L1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="M1" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="N1" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="O1" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="P1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="57" t="s">
+      <c r="Q1" s="57" t="s">
+        <v>115</v>
+      </c>
+      <c r="R1" s="58" t="s">
         <v>116</v>
       </c>
-      <c r="Q1" s="58" t="s">
-        <v>117</v>
-      </c>
-      <c r="U1" s="31"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V1" s="31"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -7591,45 +8605,45 @@
         <f>IF(ISBLANK(map_tiles!G2),"",map_tiles!G2)</f>
         <v/>
       </c>
-      <c r="I2" s="12">
-        <f>IF(ISBLANK(map_tiles!H2),"",map_tiles!H2)</f>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12">
         <v>3</v>
       </c>
-      <c r="J2" s="12" t="str">
+      <c r="K2" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!I2),"",map_tiles!I2)</f>
         <v/>
       </c>
-      <c r="K2" s="12">
+      <c r="L2" s="12">
         <f>IF(ISBLANK(map_tiles!J2),"",map_tiles!J2)</f>
         <v>1</v>
       </c>
-      <c r="L2" s="12" t="str">
+      <c r="M2" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!K2),"",map_tiles!K2)</f>
         <v/>
       </c>
-      <c r="M2" s="12" t="str">
+      <c r="N2" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!L2),"",map_tiles!L2)</f>
         <v/>
       </c>
-      <c r="N2" s="12" t="str">
+      <c r="O2" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!M2),"",map_tiles!M2)</f>
         <v/>
       </c>
-      <c r="O2" s="13" t="str">
+      <c r="P2" s="13" t="str">
         <f>IF(ISBLANK(map_tiles!N2),"",map_tiles!N2)</f>
         <v/>
       </c>
-      <c r="P2" s="11">
-        <f t="shared" ref="P2:P9" si="0">SUM(D2:O2)</f>
+      <c r="Q2" s="11">
+        <f t="shared" ref="Q2:Q9" si="0">SUM(D2:P2)</f>
         <v>5</v>
       </c>
-      <c r="Q2" s="13">
-        <f t="shared" ref="Q2:Q9" si="1">C2*P2</f>
+      <c r="R2" s="13">
+        <f t="shared" ref="R2:R9" si="1">C2*Q2</f>
         <v>0</v>
       </c>
-      <c r="T2" s="12"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U2" s="12"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -7659,45 +8673,45 @@
         <f>IF(ISBLANK(map_tiles!G3),"",map_tiles!G3)</f>
         <v/>
       </c>
-      <c r="I3" s="12" t="str">
-        <f>IF(ISBLANK(map_tiles!H3),"",map_tiles!H3)</f>
-        <v/>
-      </c>
-      <c r="J3" s="12" t="str">
+      <c r="I3" s="12"/>
+      <c r="J3" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="K3" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!I3),"",map_tiles!I3)</f>
         <v/>
       </c>
-      <c r="K3" s="12" t="str">
+      <c r="L3" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!J3),"",map_tiles!J3)</f>
         <v/>
       </c>
-      <c r="L3" s="12" t="str">
+      <c r="M3" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!K3),"",map_tiles!K3)</f>
         <v/>
       </c>
-      <c r="M3" s="12" t="str">
+      <c r="N3" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!L3),"",map_tiles!L3)</f>
         <v/>
       </c>
-      <c r="N3" s="12" t="str">
+      <c r="O3" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!M3),"",map_tiles!M3)</f>
         <v/>
       </c>
-      <c r="O3" s="13" t="str">
+      <c r="P3" s="13" t="str">
         <f>IF(ISBLANK(map_tiles!N3),"",map_tiles!N3)</f>
         <v/>
       </c>
-      <c r="P3" s="11">
+      <c r="Q3" s="11">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="Q3" s="13">
+      <c r="R3" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T3" s="12"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U3" s="12"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -7727,45 +8741,45 @@
         <f>IF(ISBLANK(map_tiles!G4),"",map_tiles!G4)</f>
         <v>1</v>
       </c>
-      <c r="I4" s="12">
-        <f>IF(ISBLANK(map_tiles!H4),"",map_tiles!H4)</f>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12">
         <v>3</v>
       </c>
-      <c r="J4" s="12" t="str">
+      <c r="K4" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!I4),"",map_tiles!I4)</f>
         <v/>
       </c>
-      <c r="K4" s="12" t="str">
+      <c r="L4" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!J4),"",map_tiles!J4)</f>
         <v/>
       </c>
-      <c r="L4" s="12">
+      <c r="M4" s="12">
         <f>IF(ISBLANK(map_tiles!K4),"",map_tiles!K4)</f>
         <v>1</v>
       </c>
-      <c r="M4" s="12" t="str">
+      <c r="N4" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!L4),"",map_tiles!L4)</f>
         <v/>
       </c>
-      <c r="N4" s="12" t="str">
+      <c r="O4" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!M4),"",map_tiles!M4)</f>
         <v/>
       </c>
-      <c r="O4" s="13" t="str">
+      <c r="P4" s="13" t="str">
         <f>IF(ISBLANK(map_tiles!N4),"",map_tiles!N4)</f>
         <v/>
       </c>
-      <c r="P4" s="11">
+      <c r="Q4" s="11">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="Q4" s="13">
+      <c r="R4" s="13">
         <f t="shared" si="1"/>
         <v>161</v>
       </c>
-      <c r="T4" s="12"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U4" s="12"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -7795,45 +8809,45 @@
         <f>IF(ISBLANK(map_tiles!G5),"",map_tiles!G5)</f>
         <v>1</v>
       </c>
-      <c r="I5" s="12">
-        <f>IF(ISBLANK(map_tiles!H5),"",map_tiles!H5)</f>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12">
         <v>3</v>
       </c>
-      <c r="J5" s="12" t="str">
+      <c r="K5" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!I5),"",map_tiles!I5)</f>
         <v/>
       </c>
-      <c r="K5" s="12" t="str">
+      <c r="L5" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!J5),"",map_tiles!J5)</f>
         <v/>
       </c>
-      <c r="L5" s="12" t="str">
+      <c r="M5" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!K5),"",map_tiles!K5)</f>
         <v/>
       </c>
-      <c r="M5" s="12" t="str">
+      <c r="N5" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!L5),"",map_tiles!L5)</f>
         <v/>
       </c>
-      <c r="N5" s="12" t="str">
+      <c r="O5" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!M5),"",map_tiles!M5)</f>
         <v/>
       </c>
-      <c r="O5" s="13" t="str">
+      <c r="P5" s="13" t="str">
         <f>IF(ISBLANK(map_tiles!N5),"",map_tiles!N5)</f>
         <v/>
       </c>
-      <c r="P5" s="11">
+      <c r="Q5" s="11">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="Q5" s="13">
+      <c r="R5" s="13">
         <f t="shared" si="1"/>
         <v>532</v>
       </c>
-      <c r="T5" s="12"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U5" s="12"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -7868,40 +8882,43 @@
         <v>1</v>
       </c>
       <c r="J6" s="12">
+        <v>1</v>
+      </c>
+      <c r="K6" s="12">
         <f>IF(ISBLANK(map_tiles!I6),"",map_tiles!I6)</f>
         <v>1</v>
       </c>
-      <c r="K6" s="12">
+      <c r="L6" s="12">
         <f>IF(ISBLANK(map_tiles!J6),"",map_tiles!J6)</f>
         <v>1</v>
       </c>
-      <c r="L6" s="12">
+      <c r="M6" s="12">
         <f>IF(ISBLANK(map_tiles!K6),"",map_tiles!K6)</f>
         <v>1</v>
       </c>
-      <c r="M6" s="12">
+      <c r="N6" s="12">
         <f>IF(ISBLANK(map_tiles!L6),"",map_tiles!L6)</f>
         <v>1</v>
       </c>
-      <c r="N6" s="12" t="str">
+      <c r="O6" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!M6),"",map_tiles!M6)</f>
         <v/>
       </c>
-      <c r="O6" s="13" t="str">
+      <c r="P6" s="13" t="str">
         <f>IF(ISBLANK(map_tiles!N6),"",map_tiles!N6)</f>
         <v/>
       </c>
-      <c r="P6" s="11">
+      <c r="Q6" s="11">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="Q6" s="13">
+        <v>9</v>
+      </c>
+      <c r="R6" s="13">
         <f t="shared" si="1"/>
-        <v>776</v>
-      </c>
-      <c r="T6" s="12"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+        <v>873</v>
+      </c>
+      <c r="U6" s="12"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -7935,41 +8952,41 @@
         <f>IF(ISBLANK(map_tiles!H7),"",map_tiles!H7)</f>
         <v/>
       </c>
-      <c r="J7" s="12" t="str">
+      <c r="J7" s="12"/>
+      <c r="K7" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!I7),"",map_tiles!I7)</f>
         <v/>
       </c>
-      <c r="K7" s="12">
-        <f>IF(ISBLANK(map_tiles!J7),"",map_tiles!J7)</f>
+      <c r="L7" s="12">
+        <v>3</v>
+      </c>
+      <c r="M7" s="12" t="str">
+        <f>IF(ISBLANK(map_tiles!K7),"",map_tiles!K7)</f>
+        <v/>
+      </c>
+      <c r="N7" s="12" t="str">
+        <f>IF(ISBLANK(map_tiles!L7),"",map_tiles!L7)</f>
+        <v/>
+      </c>
+      <c r="O7" s="12" t="str">
+        <f>IF(ISBLANK(map_tiles!M7),"",map_tiles!M7)</f>
+        <v/>
+      </c>
+      <c r="P7" s="13" t="str">
+        <f>IF(ISBLANK(map_tiles!N7),"",map_tiles!N7)</f>
+        <v/>
+      </c>
+      <c r="Q7" s="11">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="L7" s="12" t="str">
-        <f>IF(ISBLANK(map_tiles!K7),"",map_tiles!K7)</f>
-        <v/>
-      </c>
-      <c r="M7" s="12" t="str">
-        <f>IF(ISBLANK(map_tiles!L7),"",map_tiles!L7)</f>
-        <v/>
-      </c>
-      <c r="N7" s="12" t="str">
-        <f>IF(ISBLANK(map_tiles!M7),"",map_tiles!M7)</f>
-        <v/>
-      </c>
-      <c r="O7" s="13" t="str">
-        <f>IF(ISBLANK(map_tiles!N7),"",map_tiles!N7)</f>
-        <v/>
-      </c>
-      <c r="P7" s="11">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="Q7" s="13">
+      <c r="R7" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T7" s="12"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U7" s="12"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>7</v>
       </c>
@@ -8003,41 +9020,41 @@
         <f>IF(ISBLANK(map_tiles!H8),"",map_tiles!H8)</f>
         <v/>
       </c>
-      <c r="J8" s="12" t="str">
+      <c r="J8" s="12"/>
+      <c r="K8" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!I8),"",map_tiles!I8)</f>
         <v/>
       </c>
-      <c r="K8" s="12">
-        <f>IF(ISBLANK(map_tiles!J8),"",map_tiles!J8)</f>
-        <v>3</v>
-      </c>
-      <c r="L8" s="12" t="str">
+      <c r="L8" s="12">
+        <v>4</v>
+      </c>
+      <c r="M8" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!K8),"",map_tiles!K8)</f>
         <v/>
       </c>
-      <c r="M8" s="12" t="str">
+      <c r="N8" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!L8),"",map_tiles!L8)</f>
         <v/>
       </c>
-      <c r="N8" s="12" t="str">
+      <c r="O8" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!M8),"",map_tiles!M8)</f>
         <v/>
       </c>
-      <c r="O8" s="13" t="str">
+      <c r="P8" s="13" t="str">
         <f>IF(ISBLANK(map_tiles!N8),"",map_tiles!N8)</f>
         <v/>
       </c>
-      <c r="P8" s="11">
+      <c r="Q8" s="11">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="Q8" s="13">
+        <v>7</v>
+      </c>
+      <c r="R8" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T8" s="12"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U8" s="12"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="17">
         <v>8</v>
       </c>
@@ -8071,147 +9088,156 @@
         <f>IF(ISBLANK(map_tiles!H9),"",map_tiles!H9)</f>
         <v/>
       </c>
-      <c r="J9" s="12" t="str">
+      <c r="J9" s="12"/>
+      <c r="K9" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!I9),"",map_tiles!I9)</f>
         <v/>
       </c>
-      <c r="K9" s="12" t="str">
+      <c r="L9" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!J9),"",map_tiles!J9)</f>
         <v/>
       </c>
-      <c r="L9" s="12" t="str">
+      <c r="M9" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!K9),"",map_tiles!K9)</f>
         <v/>
       </c>
-      <c r="M9" s="12" t="str">
+      <c r="N9" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!L9),"",map_tiles!L9)</f>
         <v/>
       </c>
-      <c r="N9" s="12" t="str">
+      <c r="O9" s="12" t="str">
         <f>IF(ISBLANK(map_tiles!M9),"",map_tiles!M9)</f>
         <v/>
       </c>
-      <c r="O9" s="13" t="str">
+      <c r="P9" s="13" t="str">
         <f>IF(ISBLANK(map_tiles!N9),"",map_tiles!N9)</f>
         <v/>
       </c>
-      <c r="P9" s="17">
+      <c r="Q9" s="17">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="Q9" s="48">
+      <c r="R9" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T9" s="12"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U9" s="12"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="15">
-        <f>SUMPRODUCT(number,D2:D9)</f>
+        <f t="shared" ref="D10:P10" si="2">SUMPRODUCT(number,D2:D9)</f>
         <v>196</v>
       </c>
       <c r="E10" s="14">
-        <f>SUMPRODUCT(number,E2:E9)</f>
+        <f t="shared" si="2"/>
         <v>173</v>
       </c>
       <c r="F10" s="14">
-        <f>SUMPRODUCT(number,F2:F9)</f>
+        <f t="shared" si="2"/>
         <v>196</v>
       </c>
       <c r="G10" s="14">
-        <f>SUMPRODUCT(number,G2:G9)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H10" s="16">
-        <f>SUMPRODUCT(number,H2:H9)</f>
+        <f t="shared" si="2"/>
         <v>99</v>
       </c>
       <c r="I10" s="14">
-        <f>SUMPRODUCT(number,I2:I9)</f>
-        <v>394</v>
+        <f t="shared" si="2"/>
+        <v>97</v>
       </c>
       <c r="J10" s="14">
         <f>SUMPRODUCT(number,J2:J9)</f>
+        <v>394</v>
+      </c>
+      <c r="K10" s="14">
+        <f t="shared" si="2"/>
         <v>97</v>
       </c>
-      <c r="K10" s="14">
-        <f>SUMPRODUCT(number,K2:K9)</f>
+      <c r="L10" s="14">
+        <f t="shared" si="2"/>
         <v>97</v>
       </c>
-      <c r="L10" s="14">
-        <f>SUMPRODUCT(number,L2:L9)</f>
+      <c r="M10" s="14">
+        <f t="shared" si="2"/>
         <v>120</v>
       </c>
-      <c r="M10" s="14">
-        <f>SUMPRODUCT(number,M2:M9)</f>
+      <c r="N10" s="14">
+        <f t="shared" si="2"/>
         <v>97</v>
       </c>
-      <c r="N10" s="14">
-        <f>SUMPRODUCT(number,N2:N9)</f>
+      <c r="O10" s="14">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O10" s="16">
-        <f>SUMPRODUCT(number,O2:O9)</f>
+      <c r="P10" s="16">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
       <c r="D11" s="21">
-        <f t="shared" ref="D11:O11" si="2">D10/SUM(number)</f>
+        <f t="shared" ref="D11:P11" si="3">D10/SUM(number)</f>
         <v>1</v>
       </c>
       <c r="E11" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.88265306122448983</v>
       </c>
       <c r="F11" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G11" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H11" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.50510204081632648</v>
       </c>
       <c r="I11" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>0.49489795918367346</v>
+      </c>
+      <c r="J11" s="19">
+        <f>J10/SUM(number)</f>
         <v>2.010204081632653</v>
       </c>
-      <c r="J11" s="19">
-        <f t="shared" si="2"/>
+      <c r="K11" s="19">
+        <f t="shared" si="3"/>
         <v>0.49489795918367346</v>
       </c>
-      <c r="K11" s="19">
-        <f t="shared" si="2"/>
+      <c r="L11" s="19">
+        <f t="shared" si="3"/>
         <v>0.49489795918367346</v>
       </c>
-      <c r="L11" s="19">
-        <f t="shared" si="2"/>
+      <c r="M11" s="19">
+        <f t="shared" si="3"/>
         <v>0.61224489795918369</v>
       </c>
-      <c r="M11" s="19">
-        <f t="shared" si="2"/>
+      <c r="N11" s="19">
+        <f t="shared" si="3"/>
         <v>0.49489795918367346</v>
       </c>
-      <c r="N11" s="19">
-        <f t="shared" si="2"/>
+      <c r="O11" s="19">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O11" s="20">
-        <f t="shared" si="2"/>
+      <c r="P11" s="20">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>